<commit_message>
refacto tournament registration writter
</commit_message>
<xml_diff>
--- a/src/main/resources/output.xlsx
+++ b/src/main/resources/output.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kekeb\Documents\ESGI\5eme_annee\projet_annuel\ASCL-BACKEND\src\main\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{53D2BD6F-3018-45B1-AD14-2C781C30A098}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5445011D-BC6B-4AD0-AE70-E1A04BDB804E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Résumé" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="38">
   <si>
     <t>Tournois :</t>
   </si>
@@ -40,25 +40,37 @@
     <t>Type :</t>
   </si>
   <si>
-    <t>Joueur 2</t>
-  </si>
-  <si>
     <t>Numéro</t>
   </si>
   <si>
-    <t>Joueur 1</t>
-  </si>
-  <si>
-    <t>Findes inscriptions :</t>
-  </si>
-  <si>
     <t>Fin du tournois :</t>
   </si>
   <si>
     <t>Début du tournois :</t>
   </si>
   <si>
+    <t>Fin des inscriptions :</t>
+  </si>
+  <si>
+    <t>Joueur 1 (Prénom NOM)</t>
+  </si>
+  <si>
+    <t>Joueur 2  (Prénom NOM)</t>
+  </si>
+  <si>
     <t>Lyon</t>
+  </si>
+  <si>
+    <t>DOUBLE</t>
+  </si>
+  <si>
+    <t>2023-05-30</t>
+  </si>
+  <si>
+    <t>2023-06-01</t>
+  </si>
+  <si>
+    <t>2023-06-02</t>
   </si>
   <si>
     <t>azerty UIOP</t>
@@ -207,7 +219,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -222,6 +234,7 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="14" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -505,13 +518,13 @@
   <dimension ref="A1:B7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G8" sqref="G8"/>
+      <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" bestFit="true" customWidth="true" width="22.44140625" collapsed="false"/>
-    <col min="2" max="2" customWidth="true" width="8.6640625" collapsed="false"/>
+    <col min="2" max="2" customWidth="true" width="12.44140625" collapsed="false"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
@@ -526,15 +539,17 @@
       <c r="A2" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B2" t="n">
-        <v>20.0</v>
+      <c r="B2" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="1"/>
+      <c r="B3" t="n">
+        <v>20.0</v>
+      </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
@@ -548,24 +563,24 @@
       <c r="A5" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B5" t="n">
-        <v>45076.96634259259</v>
+      <c r="B5" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="B6" t="n">
-        <v>45078.96605324074</v>
+        <v>6</v>
+      </c>
+      <c r="B6" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="B7" t="n">
-        <v>45079.96623842593</v>
+        <v>5</v>
+      </c>
+      <c r="B7" t="s">
+        <v>14</v>
       </c>
     </row>
   </sheetData>
@@ -579,25 +594,25 @@
   <dimension ref="A1:C13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" bestFit="true" customWidth="true" style="2" width="10.109375" collapsed="false"/>
-    <col min="2" max="2" customWidth="true" style="2" width="13.0" collapsed="false"/>
-    <col min="3" max="3" customWidth="true" style="2" width="15.33203125" collapsed="false"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" style="2" width="21.6640625" collapsed="false"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" style="2" width="22.109375" collapsed="false"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="C1" s="5" t="s">
-        <v>4</v>
+        <v>9</v>
       </c>
     </row>
     <row r="2">
@@ -605,10 +620,10 @@
         <v>17.0</v>
       </c>
       <c r="B2" t="s">
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="C2" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
     </row>
     <row r="3">
@@ -616,10 +631,10 @@
         <v>18.0</v>
       </c>
       <c r="B3" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="C3" t="s">
-        <v>14</v>
+        <v>18</v>
       </c>
     </row>
     <row r="4">
@@ -627,10 +642,10 @@
         <v>19.0</v>
       </c>
       <c r="B4" t="s">
-        <v>15</v>
+        <v>19</v>
       </c>
       <c r="C4" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
     </row>
     <row r="5">
@@ -638,10 +653,10 @@
         <v>20.0</v>
       </c>
       <c r="B5" t="s">
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="C5" t="s">
-        <v>18</v>
+        <v>22</v>
       </c>
     </row>
     <row r="6">
@@ -649,10 +664,10 @@
         <v>21.0</v>
       </c>
       <c r="B6" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="C6" t="s">
-        <v>20</v>
+        <v>24</v>
       </c>
     </row>
     <row r="7">
@@ -660,10 +675,10 @@
         <v>22.0</v>
       </c>
       <c r="B7" t="s">
-        <v>21</v>
+        <v>25</v>
       </c>
       <c r="C7" t="s">
-        <v>22</v>
+        <v>26</v>
       </c>
     </row>
     <row r="8">
@@ -671,10 +686,10 @@
         <v>23.0</v>
       </c>
       <c r="B8" t="s">
-        <v>23</v>
+        <v>27</v>
       </c>
       <c r="C8" t="s">
-        <v>24</v>
+        <v>28</v>
       </c>
     </row>
     <row r="9">
@@ -682,10 +697,10 @@
         <v>24.0</v>
       </c>
       <c r="B9" t="s">
-        <v>24</v>
+        <v>28</v>
       </c>
       <c r="C9" t="s">
-        <v>25</v>
+        <v>29</v>
       </c>
     </row>
     <row r="10">
@@ -693,10 +708,10 @@
         <v>25.0</v>
       </c>
       <c r="B10" t="s">
-        <v>26</v>
+        <v>30</v>
       </c>
       <c r="C10" t="s">
-        <v>27</v>
+        <v>31</v>
       </c>
     </row>
     <row r="11">
@@ -704,10 +719,10 @@
         <v>26.0</v>
       </c>
       <c r="B11" t="s">
-        <v>28</v>
+        <v>32</v>
       </c>
       <c r="C11" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
     </row>
     <row r="12">
@@ -715,10 +730,10 @@
         <v>27.0</v>
       </c>
       <c r="B12" t="s">
-        <v>30</v>
+        <v>34</v>
       </c>
       <c r="C12" t="s">
-        <v>31</v>
+        <v>35</v>
       </c>
     </row>
     <row r="13">
@@ -726,10 +741,10 @@
         <v>28.0</v>
       </c>
       <c r="B13" t="s">
-        <v>32</v>
+        <v>36</v>
       </c>
       <c r="C13" t="s">
-        <v>33</v>
+        <v>37</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
TournamentRegistrationWriter : fix date format
</commit_message>
<xml_diff>
--- a/src/main/resources/output.xlsx
+++ b/src/main/resources/output.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kekeb\Documents\ESGI\5eme_annee\projet_annuel\ASCL-BACKEND\src\main\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5445011D-BC6B-4AD0-AE70-E1A04BDB804E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AF5A5229-CF00-444F-AFA3-C8260DC85F16}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
   <si>
     <t>Tournois :</t>
   </si>
@@ -61,85 +61,16 @@
     <t>Lyon</t>
   </si>
   <si>
-    <t>DOUBLE</t>
-  </si>
-  <si>
-    <t>2023-05-30</t>
-  </si>
-  <si>
-    <t>2023-06-01</t>
-  </si>
-  <si>
-    <t>2023-06-02</t>
-  </si>
-  <si>
-    <t>azerty UIOP</t>
-  </si>
-  <si>
-    <t>test1 TEST1</t>
-  </si>
-  <si>
-    <t>test2 TEST2</t>
-  </si>
-  <si>
-    <t>test3 TEST3</t>
-  </si>
-  <si>
-    <t>test5 TEST5</t>
-  </si>
-  <si>
-    <t>test6 TEST6</t>
-  </si>
-  <si>
-    <t>test7 TEST7</t>
-  </si>
-  <si>
-    <t>test4 TEST4</t>
-  </si>
-  <si>
-    <t>test8 TEST8</t>
-  </si>
-  <si>
-    <t>test9 TEST9</t>
-  </si>
-  <si>
-    <t>test10 TEST10</t>
-  </si>
-  <si>
-    <t>test13 TEST13</t>
-  </si>
-  <si>
-    <t>test14 TEST14</t>
-  </si>
-  <si>
-    <t>test15 TEST15</t>
-  </si>
-  <si>
-    <t>test16 TEST16</t>
-  </si>
-  <si>
-    <t>test17 TEST17</t>
-  </si>
-  <si>
-    <t>test18 TEST18</t>
-  </si>
-  <si>
-    <t>erger ERGERG</t>
-  </si>
-  <si>
-    <t>tert ERTER</t>
-  </si>
-  <si>
-    <t>Jean PIERRE</t>
-  </si>
-  <si>
-    <t>test TEST</t>
-  </si>
-  <si>
-    <t>Alyssia BERVIN</t>
-  </si>
-  <si>
-    <t>Catherine GENEVE</t>
+    <t>SIMPLE</t>
+  </si>
+  <si>
+    <t>2023-07-08 01:59:00.0</t>
+  </si>
+  <si>
+    <t>2023-07-09 11:00:00.0</t>
+  </si>
+  <si>
+    <t>2023-07-09 20:00:00.0</t>
   </si>
 </sst>
 </file>
@@ -524,7 +455,7 @@
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" bestFit="true" customWidth="true" width="22.44140625" collapsed="false"/>
-    <col min="2" max="2" customWidth="true" width="12.44140625" collapsed="false"/>
+    <col min="2" max="2" customWidth="true" width="19.88671875" collapsed="false"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
@@ -548,7 +479,7 @@
         <v>1</v>
       </c>
       <c r="B3" t="n">
-        <v>20.0</v>
+        <v>15.0</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
@@ -556,7 +487,7 @@
         <v>2</v>
       </c>
       <c r="B4" t="n">
-        <v>13.0</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
@@ -591,7 +522,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B4FB65EB-7D7A-4EDC-936B-3911A23C705F}">
-  <dimension ref="A1:C13"/>
+  <dimension ref="A1:C1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
@@ -615,138 +546,6 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2">
-      <c r="A2" t="n">
-        <v>17.0</v>
-      </c>
-      <c r="B2" t="s">
-        <v>15</v>
-      </c>
-      <c r="C2" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="n">
-        <v>18.0</v>
-      </c>
-      <c r="B3" t="s">
-        <v>17</v>
-      </c>
-      <c r="C3" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="n">
-        <v>19.0</v>
-      </c>
-      <c r="B4" t="s">
-        <v>19</v>
-      </c>
-      <c r="C4" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="n">
-        <v>20.0</v>
-      </c>
-      <c r="B5" t="s">
-        <v>21</v>
-      </c>
-      <c r="C5" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="n">
-        <v>21.0</v>
-      </c>
-      <c r="B6" t="s">
-        <v>23</v>
-      </c>
-      <c r="C6" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="n">
-        <v>22.0</v>
-      </c>
-      <c r="B7" t="s">
-        <v>25</v>
-      </c>
-      <c r="C7" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" t="n">
-        <v>23.0</v>
-      </c>
-      <c r="B8" t="s">
-        <v>27</v>
-      </c>
-      <c r="C8" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" t="n">
-        <v>24.0</v>
-      </c>
-      <c r="B9" t="s">
-        <v>28</v>
-      </c>
-      <c r="C9" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" t="n">
-        <v>25.0</v>
-      </c>
-      <c r="B10" t="s">
-        <v>30</v>
-      </c>
-      <c r="C10" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" t="n">
-        <v>26.0</v>
-      </c>
-      <c r="B11" t="s">
-        <v>32</v>
-      </c>
-      <c r="C11" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="12">
-      <c r="A12" t="n">
-        <v>27.0</v>
-      </c>
-      <c r="B12" t="s">
-        <v>34</v>
-      </c>
-      <c r="C12" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="13">
-      <c r="A13" t="n">
-        <v>28.0</v>
-      </c>
-      <c r="B13" t="s">
-        <v>36</v>
-      </c>
-      <c r="C13" t="s">
-        <v>37</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>